<commit_message>
Improvement in instruction / Control lines
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Instruction format" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>OP CODE</t>
   </si>
@@ -38,9 +37,6 @@
     <t>NOT USED</t>
   </si>
   <si>
-    <t>4 bits</t>
-  </si>
-  <si>
     <t>DATA</t>
   </si>
   <si>
@@ -51,6 +47,33 @@
   </si>
   <si>
     <t>12 bits</t>
+  </si>
+  <si>
+    <t>7 bits</t>
+  </si>
+  <si>
+    <t>Imediate</t>
+  </si>
+  <si>
+    <t>By Register</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>Direct By Register</t>
+  </si>
+  <si>
+    <t>9 bits</t>
+  </si>
+  <si>
+    <t>IR width = 24 bits</t>
+  </si>
+  <si>
+    <t>[RR3] Hi</t>
+  </si>
+  <si>
+    <t>[RR3] Lo</t>
   </si>
 </sst>
 </file>
@@ -74,15 +97,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -90,11 +125,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +199,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -418,112 +547,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="4" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
+  <mergeCells count="9">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
V.0.4.0 - two instructions already working
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -67,13 +67,13 @@
     <t>9 bits</t>
   </si>
   <si>
-    <t>IR width = 24 bits</t>
-  </si>
-  <si>
     <t>[RR3] Hi</t>
   </si>
   <si>
     <t>[RR3] Lo</t>
+  </si>
+  <si>
+    <t>IR width = 24 bits (3x 8 bit)</t>
   </si>
 </sst>
 </file>
@@ -204,31 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -241,6 +217,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A4:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,187 +563,187 @@
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="E14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="F15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G15" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
v.0.5.0 One more instruction working
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Instruction format" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>OP CODE</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>IR width = 24 bits (3x 8 bit)</t>
+  </si>
+  <si>
+    <t>JACA-2 Instructions Format</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H15"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +567,11 @@
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
v.0.7.0 74181 ALU added and working !
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -58,9 +58,6 @@
     <t>By Register</t>
   </si>
   <si>
-    <t>Indirect</t>
-  </si>
-  <si>
     <t>Direct By Register</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>JACA-2 Instructions Format</t>
+  </si>
+  <si>
+    <t>Direct</t>
   </si>
 </sst>
 </file>
@@ -219,6 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,7 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +554,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,23 +568,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>20</v>
+      <c r="B2" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -593,13 +593,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
@@ -615,11 +615,11 @@
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -640,11 +640,11 @@
       <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -659,11 +659,11 @@
       <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="16" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -677,10 +677,10 @@
       <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
         <v>7</v>
@@ -693,10 +693,10 @@
       <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="11"/>
       <c r="G12" s="8" t="s">
         <v>9</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>0</v>
@@ -713,15 +713,15 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -737,10 +737,10 @@
       <c r="E15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="16"/>
+      <c r="F15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Changes on structure of OUT instr to accomodate LED Matrix
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +554,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v.0.12.3 Small changes in circuit / Restore point before big changes
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>OP CODE</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Direct</t>
+  </si>
+  <si>
+    <t>// ADDR can be expanded to 15 bits (32 K words)</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,12 +570,12 @@
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
@@ -582,7 +585,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
@@ -604,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
         <v>1</v>
@@ -620,14 +623,17 @@
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="F7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -648,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="8" t="s">
         <v>1</v>
@@ -667,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -686,7 +692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
@@ -702,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -723,7 +729,7 @@
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="8" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Small changes in docs / Test program reassembled
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>OP CODE</t>
   </si>
@@ -55,31 +55,28 @@
     <t>Imediate</t>
   </si>
   <si>
-    <t>By Register</t>
+    <t>IR width = 24 bits (3x 8 bit)</t>
+  </si>
+  <si>
+    <t>JACA-2 Instructions Format</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>// ADDR can be expanded to 15 bits (32 K words)</t>
+  </si>
+  <si>
+    <t>Indirect By Register</t>
+  </si>
+  <si>
+    <t>15 bits</t>
   </si>
   <si>
     <t>Direct By Register</t>
   </si>
   <si>
-    <t>9 bits</t>
-  </si>
-  <si>
-    <t>[RR3] Hi</t>
-  </si>
-  <si>
-    <t>[RR3] Lo</t>
-  </si>
-  <si>
-    <t>IR width = 24 bits (3x 8 bit)</t>
-  </si>
-  <si>
-    <t>JACA-2 Instructions Format</t>
-  </si>
-  <si>
-    <t>Direct</t>
-  </si>
-  <si>
-    <t>// ADDR can be expanded to 15 bits (32 K words)</t>
+    <t>Address is implict in H and L registers</t>
   </si>
 </sst>
 </file>
@@ -229,25 +226,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -557,7 +554,7 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,12 +569,12 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -587,7 +584,7 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -598,11 +595,11 @@
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
@@ -618,14 +615,14 @@
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -635,7 +632,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
@@ -649,8 +646,8 @@
       <c r="E8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="15" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -668,8 +665,8 @@
       <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="17" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -686,7 +683,7 @@
       <c r="D11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
         <v>7</v>
@@ -702,7 +699,7 @@
       <c r="D12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="11"/>
       <c r="G12" s="8" t="s">
         <v>9</v>
@@ -710,7 +707,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>0</v>
@@ -718,16 +715,15 @@
       <c r="C14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="20"/>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -737,22 +733,18 @@
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="17"/>
+      <c r="D15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
     <mergeCell ref="B4:G4"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="E5:G5"/>

</xml_diff>

<commit_message>
v.0.15.0 - Led Matrix output added. Not 100% functional. Will need reassembly in programs, as instr. OUT changed parameters
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,31 +221,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -267,7 +268,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,9 +306,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,9 +341,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,9 +393,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,35 +589,35 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="2.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -595,16 +630,16 @@
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
         <v>1</v>
@@ -615,22 +650,22 @@
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="F7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -643,15 +678,15 @@
       <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="20" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="8" t="s">
         <v>1</v>
@@ -666,11 +701,11 @@
         <v>10</v>
       </c>
       <c r="F9" s="17"/>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -680,16 +715,16 @@
       <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
@@ -705,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -715,17 +750,17 @@
       <c r="C14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="20"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
       <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="8" t="s">
         <v>1</v>
@@ -738,7 +773,7 @@
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
CSCompiler - If instruction (still not working)
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -41,9 +40,6 @@
     <t>DATA</t>
   </si>
   <si>
-    <t>(least significant bit)</t>
-  </si>
-  <si>
     <t>8 bits</t>
   </si>
   <si>
@@ -78,12 +74,15 @@
   </si>
   <si>
     <t>Address is implict in H and L registers</t>
+  </si>
+  <si>
+    <t>(least significant bit) --&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,7 +267,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,9 +305,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,26 +340,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,26 +375,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,27 +554,30 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="2.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -619,7 +587,7 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -635,9 +603,7 @@
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
-      <c r="H5" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -651,13 +617,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -667,7 +633,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
@@ -698,16 +664,16 @@
         <v>3</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>0</v>
@@ -732,17 +698,17 @@
         <v>3</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="11"/>
       <c r="G12" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>0</v>
@@ -757,7 +723,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -769,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>

</xml_diff>

<commit_message>
Assembler. v0.1.0 All instructions working. Next step: labels
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/ISA.xlsx
+++ b/2nd gen - 8 bit cpu/ISA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions format" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>OP CODE</t>
   </si>
@@ -70,19 +70,31 @@
     <t>15 bits</t>
   </si>
   <si>
-    <t>Direct By Register</t>
-  </si>
-  <si>
     <t>Address is implict in H and L registers</t>
   </si>
   <si>
     <t>(least significant bit) --&gt;</t>
+  </si>
+  <si>
+    <t>By Register</t>
+  </si>
+  <si>
+    <t>e.g. LD A, [0x00c0]</t>
+  </si>
+  <si>
+    <t>e.g. LD A, C</t>
+  </si>
+  <si>
+    <t>e.g. LD H, 0xff</t>
+  </si>
+  <si>
+    <t>e.g. LD A, [HL]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,6 +258,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -265,9 +283,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,9 +323,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,9 +358,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,9 +410,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,17 +606,18 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="2.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -572,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -604,6 +657,9 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="4"/>
+      <c r="I5" s="23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -630,10 +686,11 @@
       <c r="A7" s="5"/>
       <c r="F7" s="5"/>
       <c r="H7" s="4"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
@@ -650,6 +707,9 @@
       <c r="F8" s="14"/>
       <c r="G8" s="15" t="s">
         <v>7</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -670,6 +730,10 @@
       <c r="G9" s="18" t="s">
         <v>8</v>
       </c>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -689,6 +753,9 @@
       <c r="G11" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="I11" s="23" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
@@ -705,6 +772,10 @@
       <c r="G12" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I12" s="23"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -723,7 +794,10 @@
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -740,6 +814,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
+      <c r="I15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>